<commit_message>
Remove absence section and put it in the ind quest
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3449" uniqueCount="1814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3457" uniqueCount="1822">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -5445,16 +5445,28 @@
     <t xml:space="preserve">Je, mwanakaya huyu amekuwa hayupo mara tatu</t>
   </si>
   <si>
+    <t xml:space="preserve">absent_retry_three_times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please attempt to find this household member 3 times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por favor faça 3 tentativas para encontrar este membro do agregado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tafadhali jaribu kumtafuta mwanakaya huyu mara 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">absent_skip</t>
   </si>
   <si>
-    <t xml:space="preserve">This member will be skipped</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Este membro será ignorado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mwanakaya huyu atarukwa</t>
+    <t xml:space="preserve">This household member will be ignored. Please fill out the Refusal and Absence form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este membro será ignorado. Por favor preencha o formulario de Recusas e Ausencias"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mwanakaya huyu atarukwa. Tafadhali jaza fomu ya Kukataa na Kutokuwepo</t>
   </si>
   <si>
     <t xml:space="preserve">ind_participation_q</t>
@@ -5467,6 +5479,18 @@
   </si>
   <si>
     <t xml:space="preserve">Je mwanakaya huyu atashiriki katika dodosa la mtu binafsi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ind_present_q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is this household member present at the time of the visit?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este membro do agregado esta presente no memento da visita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je mwanakaya huyu yupo wakati wa tembeleo?</t>
   </si>
 </sst>
 </file>
@@ -5650,7 +5674,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5735,7 +5759,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5857,9 +5901,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.05078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="5.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="5.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6908,19 +6952,19 @@
       <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.05078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="6.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="7.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="6.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="6.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8417,13 +8461,13 @@
       <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.05078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="7.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="6.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13697,21 +13741,21 @@
   </sheetPr>
   <dimension ref="A1:Y761"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.05078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="5.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="6.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31412,17 +31456,17 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.05078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="5.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="5.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32553,19 +32597,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ494"/>
+  <dimension ref="A1:AMJ496"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="C493" activeCellId="0" sqref="C493"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.9375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="22.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="24.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="7.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="22.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="6.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41398,22 +41442,72 @@
       <c r="AMI493" s="0"/>
       <c r="AMJ493" s="0"/>
     </row>
-    <row r="494" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="494" s="23" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A494" s="21" t="s">
         <v>1810</v>
       </c>
-      <c r="B494" s="16" t="s">
+      <c r="B494" s="22" t="s">
         <v>1811</v>
       </c>
-      <c r="C494" s="16" t="s">
+      <c r="C494" s="22" t="s">
         <v>1812</v>
       </c>
-      <c r="D494" s="16" t="s">
+      <c r="D494" s="22" t="s">
         <v>1813</v>
       </c>
+      <c r="E494" s="21"/>
+      <c r="F494" s="21"/>
+      <c r="G494" s="21"/>
+      <c r="H494" s="21"/>
+      <c r="I494" s="21"/>
+      <c r="J494" s="21"/>
+      <c r="K494" s="21"/>
+      <c r="L494" s="21"/>
+      <c r="M494" s="21"/>
+      <c r="N494" s="21"/>
+      <c r="O494" s="21"/>
+      <c r="P494" s="21"/>
+      <c r="Q494" s="21"/>
+      <c r="R494" s="21"/>
+      <c r="S494" s="21"/>
+      <c r="T494" s="21"/>
+      <c r="U494" s="21"/>
+      <c r="V494" s="21"/>
+      <c r="W494" s="21"/>
+      <c r="X494" s="21"/>
+      <c r="Y494" s="21"/>
+      <c r="Z494" s="21"/>
+    </row>
+    <row r="495" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A495" s="24" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B495" s="16" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C495" s="16" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D495" s="16" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="496" s="26" customFormat="true" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="25" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B496" s="22" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C496" s="22" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D496" s="22" t="s">
+        <v>1821</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D5 B384:D392 B396:D396 B399:D425 B495:B1048576 C127:D344 C353:D353 C451:D474 D495:D1048576 C485:D486 C355:D358 C495:C1048576 C367:D367 C6:D64 C375:C376 B485:B489 C488:C489 B490:D491 B127:B483 C378:D450 C350:D350 B6:B125 C69:D125">
+  <conditionalFormatting sqref="B1:D5 B384:D392 B396:D396 B399:D425 B497:B1048576 C127:D344 C353:D353 C451:D474 D497:D1048576 C485:D486 C355:D358 C497:C1048576 C367:D367 C6:D64 C375:C376 B485:B489 C488:C489 B490:D491 B127:B483 C378:D450 C350:D350 B6:B125 C69:D125">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>